<commit_message>
New directions to include 21.1 KMs. Fixed the sorting issue on channel and the display issue on the titile.
</commit_message>
<xml_diff>
--- a/HMDirections.xlsx
+++ b/HMDirections.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="10KDirections.xls" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Leg</t>
   </si>
@@ -103,7 +103,13 @@
     <t>Make a right onto main road ( stay right side of the road)</t>
   </si>
   <si>
-    <t>Exit the gate and proceed straight to Adarsh Clubhouse Road ( stay left side of the road)</t>
+    <t>Exit the Phase 3 exit gate and take sharp right towards Adarsh Back exit</t>
+  </si>
+  <si>
+    <t>At the Adarsh Back exit gate, take Uturn and come towards Adarsh CLUB house gate</t>
+  </si>
+  <si>
+    <t>Take a Right on to Adarsh CLUB house gate</t>
   </si>
 </sst>
 </file>
@@ -925,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -973,7 +979,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A12" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3">
@@ -991,7 +997,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <f>A3+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4">
@@ -1009,7 +1015,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5">
@@ -1027,7 +1033,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6">
@@ -1045,7 +1051,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7">
@@ -1065,7 +1071,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8">
@@ -1085,7 +1091,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9">
@@ -1103,38 +1109,38 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10">
-        <v>12.921939999999999</v>
+        <v>12.91943</v>
       </c>
       <c r="C10">
-        <v>77.694739999999996</v>
+        <v>77.696600000000004</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E10">
-        <v>2.14</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <f t="shared" ref="A11:A57" si="0">A10+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11">
-        <v>12.92216</v>
+        <v>12.919499999999999</v>
       </c>
       <c r="C11">
-        <v>77.687989999999999</v>
+        <v>77.694689999999994</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E11">
-        <v>2.88</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1143,942 +1149,1022 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>12.92008</v>
+        <v>12.921939999999999</v>
       </c>
       <c r="C12">
-        <v>77.687929999999994</v>
+        <v>77.694739999999996</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12">
-        <v>3.12</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A13:A61" si="1">A12+1</f>
         <v>12</v>
       </c>
       <c r="B13">
-        <v>12.920159999999999</v>
+        <v>12.92216</v>
       </c>
       <c r="C13">
-        <v>77.685490000000001</v>
+        <v>77.687989999999999</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E13">
-        <v>3.38</v>
+        <v>3.31</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14">
-        <v>12.92844</v>
+        <v>12.92008</v>
       </c>
       <c r="C14">
-        <v>77.684740000000005</v>
+        <v>77.687929999999994</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14">
-        <v>4.41</v>
+        <v>3.54</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15">
-        <v>12.92225</v>
+        <v>12.920159999999999</v>
       </c>
       <c r="C15">
-        <v>77.685580000000002</v>
+        <v>77.685490000000001</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E15">
-        <v>5.21</v>
+        <v>3.84</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16">
-        <v>12.922359999999999</v>
+        <v>12.92844</v>
       </c>
       <c r="C16">
-        <v>77.683040000000005</v>
+        <v>77.684740000000005</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E16">
-        <v>5.49</v>
+        <v>4.8499999999999996</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17">
-        <v>12.921810000000001</v>
+        <v>12.92225</v>
       </c>
       <c r="C17">
-        <v>77.683000000000007</v>
+        <v>77.685580000000002</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17">
-        <v>5.55</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18">
-        <v>12.92173</v>
+        <v>12.922359999999999</v>
       </c>
       <c r="C18">
-        <v>77.685280000000006</v>
+        <v>77.683040000000005</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E18">
-        <v>5.8</v>
+        <v>5.92</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19">
-        <v>12.92225</v>
+        <v>12.921810000000001</v>
       </c>
       <c r="C19">
-        <v>77.685580000000002</v>
+        <v>77.683000000000007</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E19">
-        <v>5.9</v>
+        <v>5.98</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20">
-        <v>12.920159999999999</v>
+        <v>12.92173</v>
       </c>
       <c r="C20">
-        <v>77.685490000000001</v>
+        <v>77.685280000000006</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E20">
-        <v>6.13</v>
+        <v>6.24</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21">
-        <v>12.91872</v>
+        <v>12.92225</v>
       </c>
       <c r="C21">
-        <v>77.685500000000005</v>
+        <v>77.685580000000002</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E21">
-        <v>6.29</v>
+        <v>6.33</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22">
-        <v>12.91696</v>
+        <v>12.920159999999999</v>
       </c>
       <c r="C22">
-        <v>77.689419999999998</v>
+        <v>77.685490000000001</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22">
-        <v>6.76</v>
+        <v>6.56</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23">
-        <v>12.91541</v>
+        <v>12.91872</v>
       </c>
       <c r="C23">
-        <v>77.68929</v>
+        <v>77.685500000000005</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
       </c>
       <c r="E23">
-        <v>6.94</v>
+        <v>6.72</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24">
-        <v>12.915520000000001</v>
+        <v>12.91696</v>
       </c>
       <c r="C24">
-        <v>77.698639999999997</v>
+        <v>77.689419999999998</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E24">
-        <v>7.96</v>
+        <v>7.21</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25">
-        <f>B23</f>
         <v>12.91541</v>
       </c>
       <c r="C25">
-        <f>C23</f>
         <v>77.68929</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E25">
-        <v>8.99</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B26">
-        <f>B22</f>
-        <v>12.91696</v>
+        <v>12.915520000000001</v>
       </c>
       <c r="C26">
-        <f>C22</f>
-        <v>77.689419999999998</v>
+        <v>77.698639999999997</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E26">
-        <v>9.17</v>
+        <v>8.39</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B27">
-        <f>B21</f>
-        <v>12.91872</v>
+        <f>B25</f>
+        <v>12.91541</v>
       </c>
       <c r="C27">
-        <f>C21</f>
-        <v>77.685500000000005</v>
+        <f>C25</f>
+        <v>77.68929</v>
       </c>
       <c r="D27" t="s">
         <v>14</v>
       </c>
       <c r="E27">
-        <v>9.64</v>
+        <v>9.39</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28">
-        <f>B20</f>
-        <v>12.920159999999999</v>
+        <f>B24</f>
+        <v>12.91696</v>
       </c>
       <c r="C28">
-        <f>C20</f>
-        <v>77.685490000000001</v>
+        <f>C24</f>
+        <v>77.689419999999998</v>
       </c>
       <c r="D28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E28">
-        <v>9.8000000000000007</v>
+        <v>9.5500000000000007</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B29">
-        <v>12.92008</v>
+        <f>B23</f>
+        <v>12.91872</v>
       </c>
       <c r="C29">
-        <v>77.687929999999994</v>
+        <f>C23</f>
+        <v>77.685500000000005</v>
       </c>
       <c r="D29" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E29">
-        <v>10.06</v>
+        <v>10.050000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B30">
-        <f>B2</f>
-        <v>12.9198</v>
+        <f>B22</f>
+        <v>12.920159999999999</v>
       </c>
       <c r="C30">
-        <f>C2</f>
-        <v>77.68929</v>
+        <f>C22</f>
+        <v>77.685490000000001</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E30">
-        <v>10.199999999999999</v>
+        <v>10.210000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B31">
-        <f>B3</f>
+        <v>12.92008</v>
+      </c>
+      <c r="C31">
+        <v>77.687929999999994</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <f t="shared" ref="B32:D38" si="2">B2</f>
+        <v>12.9198</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>77.68929</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>10.62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="2"/>
         <v>12.91954</v>
       </c>
-      <c r="C31">
-        <f>C3</f>
+      <c r="C33">
+        <f t="shared" si="2"/>
         <v>77.694559999999996</v>
       </c>
-      <c r="D31" t="str">
+      <c r="D33" t="str">
         <f>D3</f>
         <v>Make a Right into Adarsh Palm Retreat Phase 3</v>
       </c>
-      <c r="E31">
-        <f>E30+(E3-E2)</f>
-        <v>10.78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <f>B4</f>
+      <c r="E33">
+        <f t="shared" ref="E33:E41" si="3">E32+(E3-E2)</f>
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="2"/>
         <v>12.91774</v>
       </c>
-      <c r="C32">
-        <f>C4</f>
+      <c r="C34">
+        <f t="shared" si="2"/>
         <v>77.694400000000002</v>
       </c>
-      <c r="D32" t="str">
+      <c r="D34" t="str">
         <f>D4</f>
         <v>Make a right turn into Phase 3 Main road</v>
       </c>
-      <c r="E32">
-        <f>E31+(E4-E3)</f>
-        <v>10.99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <f>B5</f>
+      <c r="E34">
+        <f t="shared" si="3"/>
+        <v>11.41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="2"/>
         <v>12.9178</v>
       </c>
-      <c r="C33">
-        <f>C5</f>
+      <c r="C35">
+        <f t="shared" si="2"/>
         <v>77.692390000000003</v>
       </c>
-      <c r="D33" t="str">
+      <c r="D35" t="str">
         <f>D5</f>
         <v>Make a left on to Lane 1S</v>
       </c>
-      <c r="E33">
-        <f>E32+(E5-E4)</f>
-        <v>11.21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <f t="shared" ref="B34:D34" si="1">B6</f>
-        <v>12.915900000000001</v>
-      </c>
-      <c r="C34">
-        <f t="shared" si="1"/>
-        <v>77.692269999999994</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" si="1"/>
-        <v>Make a U turn</v>
-      </c>
-      <c r="E34">
-        <f t="shared" ref="E34:E57" si="2">E33+(E6-E5)</f>
-        <v>11.430000000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <f t="shared" ref="B35:D35" si="3">B7</f>
-        <v>12.9178</v>
-      </c>
-      <c r="C35">
+      <c r="E35">
         <f t="shared" si="3"/>
-        <v>77.692390000000003</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" si="3"/>
-        <v>Make a right turn into the Phase 3 Main Road</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="2"/>
-        <v>11.64</v>
+        <v>11.63</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:D36" si="4">B8</f>
-        <v>12.91774</v>
+        <f t="shared" si="2"/>
+        <v>12.915900000000001</v>
       </c>
       <c r="C36">
-        <f t="shared" si="4"/>
-        <v>77.694400000000002</v>
+        <f t="shared" si="2"/>
+        <v>77.692269999999994</v>
       </c>
       <c r="D36" t="str">
-        <f t="shared" si="4"/>
-        <v>Make a left towards the Phase 3 exit gate</v>
+        <f t="shared" si="2"/>
+        <v>Make a U turn</v>
       </c>
       <c r="E36">
-        <f t="shared" si="2"/>
-        <v>11.870000000000001</v>
+        <f t="shared" si="3"/>
+        <v>11.850000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37">
-        <f t="shared" ref="B37:D37" si="5">B9</f>
-        <v>12.91954</v>
+        <f t="shared" si="2"/>
+        <v>12.9178</v>
       </c>
       <c r="C37">
-        <f t="shared" si="5"/>
-        <v>77.694559999999996</v>
+        <f t="shared" si="2"/>
+        <v>77.692390000000003</v>
       </c>
       <c r="D37" t="str">
-        <f t="shared" si="5"/>
-        <v>Exit the gate and proceed straight to Adarsh Clubhouse Road ( stay left side of the road)</v>
+        <f t="shared" si="2"/>
+        <v>Make a right turn into the Phase 3 Main Road</v>
       </c>
       <c r="E37">
-        <f t="shared" si="2"/>
-        <v>12.07</v>
+        <f t="shared" si="3"/>
+        <v>12.060000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38">
-        <f t="shared" ref="B38:D38" si="6">B10</f>
-        <v>12.921939999999999</v>
+        <f t="shared" si="2"/>
+        <v>12.91774</v>
       </c>
       <c r="C38">
-        <f t="shared" si="6"/>
-        <v>77.694739999999996</v>
+        <f t="shared" si="2"/>
+        <v>77.694400000000002</v>
       </c>
       <c r="D38" t="str">
-        <f t="shared" si="6"/>
-        <v>Make a left onto APR Villas main road  ( stay left side of the road)</v>
+        <f t="shared" si="2"/>
+        <v>Make a left towards the Phase 3 exit gate</v>
       </c>
       <c r="E38">
-        <f t="shared" si="2"/>
-        <v>12.34</v>
+        <f t="shared" si="3"/>
+        <v>12.290000000000003</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39">
-        <f t="shared" ref="B39:D39" si="7">B11</f>
-        <v>12.92216</v>
+        <f>B9</f>
+        <v>12.91954</v>
       </c>
       <c r="C39">
-        <f t="shared" si="7"/>
-        <v>77.687989999999999</v>
+        <f>C9</f>
+        <v>77.694559999999996</v>
       </c>
       <c r="D39" t="str">
-        <f t="shared" si="7"/>
-        <v>Make a left after passing the lake on your right  ( stay left side of the road)</v>
+        <f>D9</f>
+        <v>Exit the Phase 3 exit gate and take sharp right towards Adarsh Back exit</v>
       </c>
       <c r="E39">
-        <f t="shared" si="2"/>
-        <v>13.08</v>
+        <f t="shared" si="3"/>
+        <v>12.490000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40">
-        <f t="shared" ref="B40:D40" si="8">B12</f>
-        <v>12.92008</v>
+        <f>B10</f>
+        <v>12.91943</v>
       </c>
       <c r="C40">
-        <f t="shared" si="8"/>
-        <v>77.687929999999994</v>
+        <f>C10</f>
+        <v>77.696600000000004</v>
       </c>
       <c r="D40" t="str">
-        <f t="shared" si="8"/>
-        <v>Make a right onto the main road ( stay left side of the road)</v>
+        <f>D10</f>
+        <v>At the Adarsh Back exit gate, take Uturn and come towards Adarsh CLUB house gate</v>
       </c>
       <c r="E40">
-        <f t="shared" si="2"/>
-        <v>13.32</v>
+        <f t="shared" si="3"/>
+        <v>12.720000000000002</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41">
-        <f t="shared" ref="B41:D41" si="9">B13</f>
-        <v>12.920159999999999</v>
+        <f>B11</f>
+        <v>12.919499999999999</v>
       </c>
       <c r="C41">
-        <f t="shared" si="9"/>
-        <v>77.685490000000001</v>
+        <f>C11</f>
+        <v>77.694689999999994</v>
       </c>
       <c r="D41" t="str">
-        <f t="shared" si="9"/>
-        <v>Make a right at the Bay and move straight along the road  ( stay left side of the road)</v>
+        <f>D11</f>
+        <v>Take a Right on to Adarsh CLUB house gate</v>
       </c>
       <c r="E41">
-        <f t="shared" si="2"/>
-        <v>13.58</v>
+        <f t="shared" si="3"/>
+        <v>12.930000000000003</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42">
-        <f t="shared" ref="B42:D42" si="10">B14</f>
-        <v>12.92844</v>
+        <f t="shared" ref="B42:D57" si="4">B12</f>
+        <v>12.921939999999999</v>
       </c>
       <c r="C42">
-        <f t="shared" si="10"/>
-        <v>77.684740000000005</v>
+        <f t="shared" si="4"/>
+        <v>77.694739999999996</v>
       </c>
       <c r="D42" t="str">
-        <f t="shared" si="10"/>
-        <v>Take a U turn and travel back on same road - near Villa Entrance near Intel ( stay right side of the road)</v>
+        <f t="shared" si="4"/>
+        <v>Make a left onto APR Villas main road  ( stay left side of the road)</v>
       </c>
       <c r="E42">
-        <f t="shared" si="2"/>
-        <v>14.61</v>
+        <f>E39+(E12-E9)</f>
+        <v>13.200000000000003</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43">
-        <f t="shared" ref="B43:D43" si="11">B15</f>
-        <v>12.92225</v>
+        <f t="shared" si="4"/>
+        <v>12.92216</v>
       </c>
       <c r="C43">
-        <f t="shared" si="11"/>
-        <v>77.685580000000002</v>
+        <f t="shared" si="4"/>
+        <v>77.687989999999999</v>
       </c>
       <c r="D43" t="str">
-        <f t="shared" si="11"/>
-        <v>Make a right turn into the first RMZ buidling  on the right</v>
+        <f t="shared" si="4"/>
+        <v>Make a left after passing the lake on your right  ( stay left side of the road)</v>
       </c>
       <c r="E43">
-        <f t="shared" si="2"/>
-        <v>15.41</v>
+        <f t="shared" ref="E43:E61" si="5">E42+(E13-E12)</f>
+        <v>13.930000000000003</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44">
-        <f t="shared" ref="B44:D44" si="12">B16</f>
-        <v>12.922359999999999</v>
+        <f t="shared" si="4"/>
+        <v>12.92008</v>
       </c>
       <c r="C44">
-        <f t="shared" si="12"/>
-        <v>77.683040000000005</v>
+        <f t="shared" si="4"/>
+        <v>77.687929999999994</v>
       </c>
       <c r="D44" t="str">
-        <f t="shared" si="12"/>
-        <v>Make a left within RMZ</v>
+        <f t="shared" si="4"/>
+        <v>Make a right onto the main road ( stay left side of the road)</v>
       </c>
       <c r="E44">
-        <f t="shared" si="2"/>
-        <v>15.690000000000001</v>
+        <f t="shared" si="5"/>
+        <v>14.160000000000004</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45">
-        <f t="shared" ref="B45:D45" si="13">B17</f>
-        <v>12.921810000000001</v>
+        <f t="shared" si="4"/>
+        <v>12.920159999999999</v>
       </c>
       <c r="C45">
-        <f t="shared" si="13"/>
-        <v>77.683000000000007</v>
+        <f t="shared" si="4"/>
+        <v>77.685490000000001</v>
       </c>
       <c r="D45" t="str">
-        <f t="shared" si="13"/>
-        <v>Make a left within RMZ</v>
+        <f t="shared" si="4"/>
+        <v>Make a right at the Bay and move straight along the road  ( stay left side of the road)</v>
       </c>
       <c r="E45">
-        <f t="shared" si="2"/>
-        <v>15.75</v>
+        <f t="shared" si="5"/>
+        <v>14.460000000000004</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B46">
-        <f t="shared" ref="B46:D46" si="14">B18</f>
-        <v>12.92173</v>
+        <f t="shared" si="4"/>
+        <v>12.92844</v>
       </c>
       <c r="C46">
-        <f t="shared" si="14"/>
-        <v>77.685280000000006</v>
+        <f t="shared" si="4"/>
+        <v>77.684740000000005</v>
       </c>
       <c r="D46" t="str">
-        <f t="shared" si="14"/>
-        <v>Exit  RMZ  by moving zig zag, left right, left right quickly</v>
+        <f t="shared" si="4"/>
+        <v>Take a U turn and travel back on same road - near Villa Entrance near Intel ( stay right side of the road)</v>
       </c>
       <c r="E46">
-        <f t="shared" si="2"/>
-        <v>16</v>
+        <f t="shared" si="5"/>
+        <v>15.470000000000004</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B47">
-        <f t="shared" ref="B47:D47" si="15">B19</f>
+        <f t="shared" si="4"/>
         <v>12.92225</v>
       </c>
       <c r="C47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="4"/>
         <v>77.685580000000002</v>
       </c>
       <c r="D47" t="str">
-        <f t="shared" si="15"/>
-        <v>Make a right onto main road ( stay right side of the road)</v>
+        <f t="shared" si="4"/>
+        <v>Make a right turn into the first RMZ buidling  on the right</v>
       </c>
       <c r="E47">
-        <f t="shared" si="2"/>
-        <v>16.100000000000001</v>
+        <f t="shared" si="5"/>
+        <v>16.260000000000005</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B48">
-        <f t="shared" ref="B48:D48" si="16">B20</f>
-        <v>12.920159999999999</v>
+        <f t="shared" si="4"/>
+        <v>12.922359999999999</v>
       </c>
       <c r="C48">
-        <f t="shared" si="16"/>
-        <v>77.685490000000001</v>
+        <f t="shared" si="4"/>
+        <v>77.683040000000005</v>
       </c>
       <c r="D48" t="str">
-        <f t="shared" si="16"/>
-        <v>Go Straight towards the T Junction</v>
+        <f t="shared" si="4"/>
+        <v>Make a left within RMZ</v>
       </c>
       <c r="E48">
-        <f t="shared" si="2"/>
-        <v>16.330000000000002</v>
+        <f t="shared" si="5"/>
+        <v>16.540000000000006</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49">
-        <f t="shared" ref="B49:D49" si="17">B21</f>
-        <v>12.91872</v>
+        <f t="shared" si="4"/>
+        <v>12.921810000000001</v>
       </c>
       <c r="C49">
-        <f t="shared" si="17"/>
-        <v>77.685500000000005</v>
+        <f t="shared" si="4"/>
+        <v>77.683000000000007</v>
       </c>
       <c r="D49" t="str">
-        <f t="shared" si="17"/>
-        <v>Make a left</v>
+        <f t="shared" si="4"/>
+        <v>Make a left within RMZ</v>
       </c>
       <c r="E49">
-        <f t="shared" si="2"/>
-        <v>16.490000000000002</v>
+        <f t="shared" si="5"/>
+        <v>16.600000000000009</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50">
-        <f t="shared" ref="B50:D50" si="18">B22</f>
-        <v>12.91696</v>
+        <f t="shared" si="4"/>
+        <v>12.92173</v>
       </c>
       <c r="C50">
-        <f t="shared" si="18"/>
-        <v>77.689419999999998</v>
+        <f t="shared" si="4"/>
+        <v>77.685280000000006</v>
       </c>
       <c r="D50" t="str">
-        <f t="shared" si="18"/>
-        <v>Make a right</v>
+        <f t="shared" si="4"/>
+        <v>Exit  RMZ  by moving zig zag, left right, left right quickly</v>
       </c>
       <c r="E50">
-        <f t="shared" si="2"/>
-        <v>16.96</v>
+        <f t="shared" si="5"/>
+        <v>16.860000000000007</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51">
-        <f t="shared" ref="B51:D51" si="19">B23</f>
-        <v>12.91541</v>
+        <f t="shared" si="4"/>
+        <v>12.92225</v>
       </c>
       <c r="C51">
-        <f t="shared" si="19"/>
-        <v>77.68929</v>
+        <f t="shared" si="4"/>
+        <v>77.685580000000002</v>
       </c>
       <c r="D51" t="str">
-        <f t="shared" si="19"/>
-        <v>Make a left</v>
+        <f t="shared" si="4"/>
+        <v>Make a right onto main road ( stay right side of the road)</v>
       </c>
       <c r="E51">
-        <f t="shared" si="2"/>
-        <v>17.14</v>
+        <f t="shared" si="5"/>
+        <v>16.950000000000006</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B52">
-        <f t="shared" ref="B52:D52" si="20">B24</f>
-        <v>12.915520000000001</v>
+        <f t="shared" si="4"/>
+        <v>12.920159999999999</v>
       </c>
       <c r="C52">
-        <f t="shared" si="20"/>
-        <v>77.698639999999997</v>
+        <f t="shared" si="4"/>
+        <v>77.685490000000001</v>
       </c>
       <c r="D52" t="str">
-        <f t="shared" si="20"/>
-        <v>Make a U turn</v>
+        <f t="shared" si="4"/>
+        <v>Go Straight towards the T Junction</v>
       </c>
       <c r="E52">
-        <f t="shared" si="2"/>
-        <v>18.16</v>
+        <f t="shared" si="5"/>
+        <v>17.180000000000007</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B53">
-        <f t="shared" ref="B53:D53" si="21">B25</f>
-        <v>12.91541</v>
+        <f t="shared" si="4"/>
+        <v>12.91872</v>
       </c>
       <c r="C53">
-        <f t="shared" si="21"/>
-        <v>77.68929</v>
+        <f t="shared" si="4"/>
+        <v>77.685500000000005</v>
       </c>
       <c r="D53" t="str">
-        <f t="shared" si="21"/>
-        <v>Make a right</v>
+        <f t="shared" si="4"/>
+        <v>Make a left</v>
       </c>
       <c r="E53">
-        <f t="shared" si="2"/>
-        <v>19.190000000000001</v>
+        <f t="shared" si="5"/>
+        <v>17.340000000000007</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B54">
-        <f t="shared" ref="B54:D54" si="22">B26</f>
+        <f t="shared" si="4"/>
         <v>12.91696</v>
       </c>
       <c r="C54">
-        <f t="shared" si="22"/>
+        <f t="shared" si="4"/>
         <v>77.689419999999998</v>
       </c>
       <c r="D54" t="str">
-        <f t="shared" si="22"/>
-        <v>Make a left</v>
+        <f t="shared" si="4"/>
+        <v>Make a right</v>
       </c>
       <c r="E54">
-        <f t="shared" si="2"/>
-        <v>19.37</v>
+        <f t="shared" si="5"/>
+        <v>17.830000000000005</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B55">
-        <f t="shared" ref="B55:D55" si="23">B27</f>
-        <v>12.91872</v>
+        <f t="shared" si="4"/>
+        <v>12.91541</v>
       </c>
       <c r="C55">
-        <f t="shared" si="23"/>
-        <v>77.685500000000005</v>
+        <f t="shared" si="4"/>
+        <v>77.68929</v>
       </c>
       <c r="D55" t="str">
-        <f t="shared" si="23"/>
-        <v>Make a right</v>
+        <f t="shared" si="4"/>
+        <v>Make a left</v>
       </c>
       <c r="E55">
-        <f t="shared" si="2"/>
-        <v>19.840000000000003</v>
+        <f t="shared" si="5"/>
+        <v>18.020000000000007</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="B56">
-        <f t="shared" ref="B56:D56" si="24">B28</f>
-        <v>12.920159999999999</v>
+        <f t="shared" si="4"/>
+        <v>12.915520000000001</v>
       </c>
       <c r="C56">
-        <f t="shared" si="24"/>
-        <v>77.685490000000001</v>
-      </c>
-      <c r="D56" t="s">
-        <v>17</v>
+        <f t="shared" si="4"/>
+        <v>77.698639999999997</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="4"/>
+        <v>Make a U turn</v>
       </c>
       <c r="E56">
-        <f t="shared" si="2"/>
-        <v>20.000000000000004</v>
+        <f t="shared" si="5"/>
+        <v>19.010000000000005</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:D57" si="25">B29</f>
+        <f t="shared" si="4"/>
+        <v>12.91541</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="4"/>
+        <v>77.68929</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="4"/>
+        <v>Make a right</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="5"/>
+        <v>20.010000000000005</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <f t="shared" ref="B58:D61" si="6">B28</f>
+        <v>12.91696</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="6"/>
+        <v>77.689419999999998</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="6"/>
+        <v>Make a left</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="5"/>
+        <v>20.170000000000005</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="6"/>
+        <v>12.91872</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="6"/>
+        <v>77.685500000000005</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="6"/>
+        <v>Make a right</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="5"/>
+        <v>20.670000000000005</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="6"/>
+        <v>12.920159999999999</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="6"/>
+        <v>77.685490000000001</v>
+      </c>
+      <c r="D60" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="5"/>
+        <v>20.830000000000005</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="6"/>
         <v>12.92008</v>
       </c>
-      <c r="C57">
-        <f t="shared" si="25"/>
+      <c r="C61">
+        <f t="shared" si="6"/>
         <v>77.687929999999994</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D61" t="s">
         <v>18</v>
       </c>
-      <c r="E57">
-        <f t="shared" si="2"/>
-        <v>20.260000000000005</v>
+      <c r="E61">
+        <f t="shared" si="5"/>
+        <v>21.120000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>